<commit_message>
Added rda data the folder R/data and corresponding documentation
</commit_message>
<xml_diff>
--- a/inst/extdata/BIP_Landkreise.xlsx
+++ b/inst/extdata/BIP_Landkreise.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="59" documentId="8_{6C2B1499-70DE-4F7B-9141-065130F1020E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{2075BB2C-1AF9-4BE6-8A8A-F9DE53B755C3}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Kreise" sheetId="1" r:id="rId1"/>
@@ -1691,7 +1691,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D403"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
@@ -7353,7 +7353,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
@@ -7540,7 +7540,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L16" sqref="L16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>